<commit_message>
Append all except "Настройка playlist"
</commit_message>
<xml_diff>
--- a/iSpring/TestCase.xlsx
+++ b/iSpring/TestCase.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="357">
   <si>
     <t>билд</t>
   </si>
@@ -1509,6 +1509,132 @@
   </si>
   <si>
     <t xml:space="preserve">У выделенного слайда иконка c синим кружком(в ленте и колонке Advance)выделяется синим квадратом если не было выделено ранее, и наоборот. </t>
+  </si>
+  <si>
+    <t>Проверка на одном выделенном слайде</t>
+  </si>
+  <si>
+    <t>Появляется окошко с двумя выпадающими списками, в которых можно выбрать переход</t>
+  </si>
+  <si>
+    <t>Нажимаем левую кнопку мыши в столбце Branching на надписи в центре ячейки таблицы у того слайда переход у которого хотим изменить</t>
+  </si>
+  <si>
+    <t>Нажимаем левую кнопку мыши на списке под надписью Forward branching</t>
+  </si>
+  <si>
+    <t>Появляется выпадающий список с возможными переходам</t>
+  </si>
+  <si>
+    <t>Выбираем м нажимаем левую кнопку мыши</t>
+  </si>
+  <si>
+    <t>Выбранный переход сохранён и отображается в списке</t>
+  </si>
+  <si>
+    <t>Нажимаем левую кнопку мыши на списке под надписью Backward branching</t>
+  </si>
+  <si>
+    <t>Нажимаем на кнопку OK</t>
+  </si>
+  <si>
+    <t>Окно закрывается и на месте старой надписи отображается выбранный ранее переход на следующий слайд</t>
+  </si>
+  <si>
+    <t>Перевыбираем переходы, выбираем другие и нажимаем на кнопку Cancel</t>
+  </si>
+  <si>
+    <t>Не был выбран новый переход, остался старый</t>
+  </si>
+  <si>
+    <t>Нажимаем левую кнопку мыши в столбце Lock в центре ячейки таблицы у того слайда который хотим блокировать</t>
+  </si>
+  <si>
+    <t>В столбце Lock появляется изображение замка в синем квадрате и в ленте в разделе Navigation кнопка Lock выделяется синим квадартом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выделяем слайд нажитием левой кнопки мыши и в ленте в разделе  Navigation нажимаем на кнопку  Lock </t>
+  </si>
+  <si>
+    <t>Проверка на нескольких выделенном слайде</t>
+  </si>
+  <si>
+    <t>В случае если слайды имеют разные переходы то отображается картинка с надписью Multiply slides selected</t>
+  </si>
+  <si>
+    <t>Работает также как и в случае с одним слайдом, переходы устанавливаются для всех выделенных слайдов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Если слайды имеют разные переходы то в выпадающих списках будет отображаться картика с надписью </t>
+  </si>
+  <si>
+    <t>В столбце Presenter у соответсвтйющего слайда нажимаем на название докладчика(если нет то None)</t>
+  </si>
+  <si>
+    <t>Появляется выпадающий список с докладчиками</t>
+  </si>
+  <si>
+    <t>Выбираем докладчика щелчком мыши</t>
+  </si>
+  <si>
+    <t>Имя выбранного докладчика и его изображение появляется вместо старой надписи и изображения соответсвенно</t>
+  </si>
+  <si>
+    <t>В столбце Layout у соответсвующего слайда нажимаем на текст</t>
+  </si>
+  <si>
+    <t>Появляется выпадающий список с несколькими вариантами</t>
+  </si>
+  <si>
+    <t>Выбранная настройка и соответствующая ей картинка появляется вместо старой надписи и картинки соответсвенно</t>
+  </si>
+  <si>
+    <t>При щелчке вне списка</t>
+  </si>
+  <si>
+    <t>Список закрывается</t>
+  </si>
+  <si>
+    <t>В столбце Playlist у соответсвующего слайда нажимаем на текст</t>
+  </si>
+  <si>
+    <t>Появляется выпадающий список с playlist</t>
+  </si>
+  <si>
+    <t>Выбираем playlist щелчком мыши</t>
+  </si>
+  <si>
+    <t>Выбранный playlist и появляется вместо старого</t>
+  </si>
+  <si>
+    <t>Выбираем слайд и нажимаем левой кнопкой мыши на кнопку Hide slide в ленте в разделе Display slides</t>
+  </si>
+  <si>
+    <t>Картинка выбранного слайда становится светлее и над ним надпись hidden в сером скруглённом прямоугольнике</t>
+  </si>
+  <si>
+    <t>Если слайд уже скрыт то он становится видным, он не забелён и нет надписи</t>
+  </si>
+  <si>
+    <t>Нажимаем на иконку с синим кружучком в котором находится курсор</t>
+  </si>
+  <si>
+    <t>Выделить слайд и нажать на playlist в ленте в разделе Advanced</t>
+  </si>
+  <si>
+    <t>Поведение списка из ленты такое же как и в столбце Playlist</t>
+  </si>
+  <si>
+    <t>Выделить слайд и нажать на Layout  в ленте в разделе Advanced</t>
+  </si>
+  <si>
+    <t>Поведение списка из ленты такое же как и в столбце Layout</t>
+  </si>
+  <si>
+    <t>Выделить слайд и нажать на Presenter   в ленте в разделе Advanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поведение списка из ленты такое же как и в столбце Presenter </t>
   </si>
 </sst>
 </file>
@@ -1877,7 +2003,7 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2012,9 +2138,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2093,9 +2216,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2117,6 +2237,21 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2334,6 +2469,100 @@
         <a:xfrm>
           <a:off x="5819775" y="11556072"/>
           <a:ext cx="8277225" cy="3102903"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>676275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>192146</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6219825" y="16297275"/>
+          <a:ext cx="2516246" cy="1838325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>699897</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>619125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4967097" y="24050625"/>
+          <a:ext cx="2910078" cy="2171700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2652,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2678,7 +2907,7 @@
     </row>
     <row r="3" spans="1:7" ht="21">
       <c r="B3" s="17"/>
-      <c r="C3" s="71"/>
+      <c r="C3" s="70"/>
       <c r="D3" t="s">
         <v>267</v>
       </c>
@@ -2688,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="72"/>
+      <c r="C4" s="71"/>
       <c r="D4" t="s">
         <v>268</v>
       </c>
@@ -2700,7 +2929,7 @@
       <c r="B5" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C5" s="73"/>
+      <c r="C5" s="72"/>
       <c r="D5" t="s">
         <v>269</v>
       </c>
@@ -2757,7 +2986,7 @@
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
@@ -2769,7 +2998,7 @@
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
@@ -2781,7 +3010,7 @@
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="70"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
@@ -2793,7 +3022,7 @@
       <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
@@ -2805,7 +3034,7 @@
       <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="70"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
@@ -2817,7 +3046,7 @@
       <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="70"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
@@ -2833,7 +3062,7 @@
       <c r="B18" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="73"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -2843,7 +3072,7 @@
       <c r="B19" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C19" s="74"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -2853,7 +3082,7 @@
       <c r="B20" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C20" s="74"/>
+      <c r="C20" s="73"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -2863,7 +3092,7 @@
       <c r="B21" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C21" s="74"/>
+      <c r="C21" s="73"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -2883,7 +3112,7 @@
       <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="73"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
@@ -2895,7 +3124,7 @@
       <c r="B24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="74"/>
+      <c r="C24" s="73"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -2907,7 +3136,7 @@
       <c r="B25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="74"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -2919,7 +3148,7 @@
       <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="73"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -2931,7 +3160,7 @@
       <c r="B27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="74"/>
+      <c r="C27" s="73"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -2943,218 +3172,218 @@
       <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="74"/>
+      <c r="C28" s="73"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A29" s="83"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="79"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="78"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="63"/>
-      <c r="B30" s="80"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="79"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="81"/>
+      <c r="G30" s="80"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="63"/>
-      <c r="B31" s="80"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="81"/>
+      <c r="G31" s="80"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="63"/>
-      <c r="B32" s="80"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="81"/>
+      <c r="G32" s="80"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="63"/>
-      <c r="B33" s="80"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="79"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="81"/>
+      <c r="G33" s="80"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="63"/>
-      <c r="B34" s="80"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="81"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="80"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="63"/>
-      <c r="B35" s="80"/>
-      <c r="C35" s="82"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="81"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="80"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="63"/>
-      <c r="B36" s="80"/>
+      <c r="A36" s="62"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="81"/>
+      <c r="G36" s="80"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="63"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
+      <c r="A37" s="62"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
     </row>
     <row r="38" spans="1:7" s="8" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A38" s="84"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="85"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="84"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="63"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="63"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="62"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="63"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="11"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
-      <c r="G40" s="63"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="62"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="63"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="82"/>
-      <c r="G41" s="63"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="62"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="63"/>
-      <c r="B42" s="80"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="82"/>
-      <c r="G42" s="63"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="79"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="81"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="63"/>
-      <c r="B43" s="80"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="82"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="63"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="79"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="62"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="63"/>
-      <c r="B44" s="80"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="63"/>
+      <c r="A44" s="62"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="62"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="63"/>
-      <c r="B45" s="80"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="63"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="79"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="62"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="63"/>
-      <c r="B46" s="80"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="63"/>
+      <c r="A46" s="62"/>
+      <c r="B46" s="79"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="81"/>
+      <c r="F46" s="81"/>
+      <c r="G46" s="62"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="63"/>
-      <c r="B47" s="80"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="63"/>
+      <c r="A47" s="62"/>
+      <c r="B47" s="79"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="62"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="63"/>
+      <c r="A48" s="62"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="63"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="62"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="63"/>
+      <c r="A49" s="62"/>
       <c r="B49" s="11"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="63"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="62"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="63"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="11"/>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="63"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="62"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="63"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
+      <c r="A51" s="62"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
     </row>
     <row r="52" spans="1:7" ht="21">
       <c r="B52" s="17"/>
@@ -3188,58 +3417,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1">
       <c r="A2" s="49" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="47"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="47"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="47"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
     </row>
     <row r="5" spans="1:6" ht="20.25" customHeight="1">
       <c r="A5" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="71"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="70"/>
       <c r="D5" t="s">
         <v>267</v>
       </c>
-      <c r="E5" s="65"/>
+      <c r="E5" s="64"/>
       <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
-      <c r="C6" s="72"/>
+      <c r="C6" s="71"/>
       <c r="D6" t="s">
         <v>268</v>
       </c>
@@ -3248,7 +3477,7 @@
       <c r="B7" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="73"/>
+      <c r="C7" s="72"/>
       <c r="D7" t="s">
         <v>269</v>
       </c>
@@ -3283,7 +3512,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="33"/>
-      <c r="D11" s="66"/>
+      <c r="D11" s="65"/>
       <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:6">
@@ -3291,14 +3520,14 @@
         <v>34</v>
       </c>
       <c r="C12" s="33"/>
-      <c r="D12" s="66"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="75"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="37"/>
       <c r="E13" s="34"/>
     </row>
@@ -3306,15 +3535,15 @@
       <c r="B14" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="66"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="65"/>
       <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="75"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="37"/>
       <c r="E15" s="34"/>
     </row>
@@ -3322,32 +3551,32 @@
       <c r="B16" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="66"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="65"/>
       <c r="E16" s="34"/>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="66"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="34"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="75"/>
-      <c r="D18" s="66"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="65"/>
       <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="66"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="34"/>
     </row>
     <row r="20" spans="1:6" s="31" customFormat="1" ht="29.25" customHeight="1">
@@ -3365,7 +3594,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="33"/>
-      <c r="D21" s="66"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:6">
@@ -3373,7 +3602,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="33"/>
-      <c r="D22" s="66"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:6" ht="30">
@@ -3381,7 +3610,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="33"/>
-      <c r="D23" s="66" t="s">
+      <c r="D23" s="65" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="34"/>
@@ -3391,7 +3620,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="33"/>
-      <c r="D24" s="66"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="34"/>
     </row>
     <row r="25" spans="1:6" s="31" customFormat="1" ht="29.25" customHeight="1">
@@ -3408,7 +3637,7 @@
       <c r="B26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="75"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="39" t="s">
         <v>49</v>
       </c>
@@ -3418,8 +3647,8 @@
       <c r="B27" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="66"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="65"/>
       <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:6" s="31" customFormat="1" ht="29.25" customHeight="1">
@@ -3436,8 +3665,8 @@
       <c r="B29" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="66"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="65"/>
       <c r="E29" s="34"/>
     </row>
     <row r="30" spans="1:6">
@@ -3452,32 +3681,32 @@
       <c r="B31" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="66"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="65"/>
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:6">
       <c r="B32" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="66"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="34"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="75"/>
-      <c r="D33" s="66"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="65"/>
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="66"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="65"/>
       <c r="E34" s="34"/>
     </row>
     <row r="35" spans="2:5">
@@ -3492,40 +3721,40 @@
       <c r="B36" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="75"/>
-      <c r="D36" s="66"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="65"/>
       <c r="E36" s="34"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="66"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="65"/>
       <c r="E37" s="34"/>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="66"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="34"/>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="75"/>
-      <c r="D39" s="66"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="65"/>
       <c r="E39" s="34"/>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="75"/>
-      <c r="D40" s="66"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="34"/>
     </row>
     <row r="41" spans="2:5">
@@ -3540,8 +3769,8 @@
       <c r="B42" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="75"/>
-      <c r="D42" s="66" t="s">
+      <c r="C42" s="74"/>
+      <c r="D42" s="65" t="s">
         <v>66</v>
       </c>
       <c r="E42" s="34"/>
@@ -3550,32 +3779,32 @@
       <c r="B43" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="75"/>
-      <c r="D43" s="66"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="65"/>
       <c r="E43" s="34"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="75"/>
-      <c r="D44" s="66"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="65"/>
       <c r="E44" s="34"/>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="75" t="s">
         <v>69</v>
       </c>
       <c r="C45" s="33"/>
-      <c r="D45" s="66"/>
+      <c r="D45" s="65"/>
       <c r="E45" s="34"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="75"/>
-      <c r="D46" s="66" t="s">
+      <c r="C46" s="74"/>
+      <c r="D46" s="65" t="s">
         <v>71</v>
       </c>
       <c r="E46" s="34"/>
@@ -3584,8 +3813,8 @@
       <c r="B47" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="75"/>
-      <c r="D47" s="66">
+      <c r="C47" s="74"/>
+      <c r="D47" s="65">
         <v>200</v>
       </c>
       <c r="E47" s="34"/>
@@ -3594,16 +3823,16 @@
       <c r="B48" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="75"/>
-      <c r="D48" s="66"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="65"/>
       <c r="E48" s="34"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="75"/>
-      <c r="D49" s="66" t="s">
+      <c r="C49" s="74"/>
+      <c r="D49" s="65" t="s">
         <v>75</v>
       </c>
       <c r="E49" s="34"/>
@@ -3612,8 +3841,8 @@
       <c r="B50" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="75"/>
-      <c r="D50" s="66"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="65"/>
       <c r="E50" s="34"/>
     </row>
     <row r="51" spans="2:5">
@@ -3628,50 +3857,50 @@
       <c r="B52" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C52" s="75"/>
-      <c r="D52" s="66"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="65"/>
       <c r="E52" s="34"/>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="75"/>
-      <c r="D53" s="66"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="65"/>
       <c r="E53" s="34"/>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="75"/>
-      <c r="D54" s="66" t="s">
+      <c r="C54" s="74"/>
+      <c r="D54" s="65" t="s">
         <v>80</v>
       </c>
       <c r="E54" s="34"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="76" t="s">
+      <c r="B55" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="75"/>
-      <c r="D55" s="66"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="65"/>
       <c r="E55" s="34"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C56" s="75"/>
-      <c r="D56" s="66"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="65"/>
       <c r="E56" s="34"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="75"/>
-      <c r="D57" s="66">
+      <c r="C57" s="74"/>
+      <c r="D57" s="65">
         <v>200</v>
       </c>
       <c r="E57" s="34"/>
@@ -3680,8 +3909,8 @@
       <c r="B58" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C58" s="75"/>
-      <c r="D58" s="66" t="s">
+      <c r="C58" s="74"/>
+      <c r="D58" s="65" t="s">
         <v>75</v>
       </c>
       <c r="E58" s="34"/>
@@ -3690,8 +3919,8 @@
       <c r="B59" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="75"/>
-      <c r="D59" s="66"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="65"/>
       <c r="E59" s="34"/>
     </row>
     <row r="60" spans="2:5">
@@ -3706,8 +3935,8 @@
       <c r="B61" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="75"/>
-      <c r="D61" s="66" t="s">
+      <c r="C61" s="74"/>
+      <c r="D61" s="65" t="s">
         <v>86</v>
       </c>
       <c r="E61" s="34"/>
@@ -3716,16 +3945,16 @@
       <c r="B62" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="75"/>
-      <c r="D62" s="66"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="65"/>
       <c r="E62" s="34"/>
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="66" t="s">
+      <c r="C63" s="74"/>
+      <c r="D63" s="65" t="s">
         <v>89</v>
       </c>
       <c r="E63" s="34"/>
@@ -3734,8 +3963,8 @@
       <c r="B64" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="66"/>
+      <c r="C64" s="74"/>
+      <c r="D64" s="65"/>
       <c r="E64" s="34"/>
     </row>
     <row r="65" spans="1:6" s="31" customFormat="1" ht="29.25" customHeight="1">
@@ -3760,32 +3989,32 @@
       <c r="B67" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="75"/>
-      <c r="D67" s="66"/>
+      <c r="C67" s="74"/>
+      <c r="D67" s="65"/>
       <c r="E67" s="34"/>
     </row>
     <row r="68" spans="1:6">
       <c r="B68" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="75"/>
-      <c r="D68" s="66"/>
+      <c r="C68" s="74"/>
+      <c r="D68" s="65"/>
       <c r="E68" s="34"/>
     </row>
     <row r="69" spans="1:6" ht="45">
       <c r="B69" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C69" s="75"/>
-      <c r="D69" s="66"/>
+      <c r="C69" s="74"/>
+      <c r="D69" s="65"/>
       <c r="E69" s="34"/>
     </row>
     <row r="70" spans="1:6">
       <c r="B70" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C70" s="75"/>
-      <c r="D70" s="66"/>
+      <c r="C70" s="74"/>
+      <c r="D70" s="65"/>
       <c r="E70" s="34"/>
     </row>
     <row r="71" spans="1:6">
@@ -3793,7 +4022,7 @@
         <v>97</v>
       </c>
       <c r="C71" s="33"/>
-      <c r="D71" s="66"/>
+      <c r="D71" s="65"/>
       <c r="E71" s="34"/>
     </row>
     <row r="72" spans="1:6" ht="30">
@@ -3801,7 +4030,7 @@
         <v>98</v>
       </c>
       <c r="C72" s="33"/>
-      <c r="D72" s="66" t="s">
+      <c r="D72" s="65" t="s">
         <v>99</v>
       </c>
       <c r="E72" s="34"/>
@@ -3811,7 +4040,7 @@
         <v>100</v>
       </c>
       <c r="C73" s="33"/>
-      <c r="D73" s="66"/>
+      <c r="D73" s="65"/>
       <c r="E73" s="34"/>
     </row>
     <row r="74" spans="1:6">
@@ -3819,7 +4048,7 @@
         <v>101</v>
       </c>
       <c r="C74" s="33"/>
-      <c r="D74" s="66" t="s">
+      <c r="D74" s="65" t="s">
         <v>102</v>
       </c>
       <c r="E74" s="34"/>
@@ -3829,7 +4058,7 @@
         <v>103</v>
       </c>
       <c r="C75" s="33"/>
-      <c r="D75" s="66"/>
+      <c r="D75" s="65"/>
       <c r="E75" s="34"/>
     </row>
     <row r="76" spans="1:6">
@@ -3837,7 +4066,7 @@
         <v>104</v>
       </c>
       <c r="C76" s="33"/>
-      <c r="D76" s="66" t="s">
+      <c r="D76" s="65" t="s">
         <v>105</v>
       </c>
       <c r="E76" s="34"/>
@@ -3847,7 +4076,7 @@
         <v>106</v>
       </c>
       <c r="C77" s="33"/>
-      <c r="D77" s="66" t="s">
+      <c r="D77" s="65" t="s">
         <v>107</v>
       </c>
       <c r="E77" s="34"/>
@@ -3857,7 +4086,7 @@
         <v>108</v>
       </c>
       <c r="C78" s="33"/>
-      <c r="D78" s="66"/>
+      <c r="D78" s="65"/>
       <c r="E78" s="34"/>
     </row>
     <row r="79" spans="1:6">
@@ -3873,7 +4102,7 @@
         <v>110</v>
       </c>
       <c r="C80" s="33"/>
-      <c r="D80" s="66" t="s">
+      <c r="D80" s="65" t="s">
         <v>111</v>
       </c>
       <c r="E80" s="34"/>
@@ -3883,7 +4112,7 @@
         <v>112</v>
       </c>
       <c r="C81" s="33"/>
-      <c r="D81" s="66" t="s">
+      <c r="D81" s="65" t="s">
         <v>113</v>
       </c>
       <c r="E81" s="34"/>
@@ -3893,7 +4122,7 @@
         <v>114</v>
       </c>
       <c r="C82" s="33"/>
-      <c r="D82" s="66"/>
+      <c r="D82" s="65"/>
       <c r="E82" s="34"/>
     </row>
     <row r="83" spans="2:5">
@@ -3901,7 +4130,7 @@
         <v>115</v>
       </c>
       <c r="C83" s="33"/>
-      <c r="D83" s="66" t="s">
+      <c r="D83" s="65" t="s">
         <v>116</v>
       </c>
       <c r="E83" s="34"/>
@@ -3911,7 +4140,7 @@
         <v>117</v>
       </c>
       <c r="C84" s="33"/>
-      <c r="D84" s="66"/>
+      <c r="D84" s="65"/>
       <c r="E84" s="34"/>
     </row>
     <row r="85" spans="2:5">
@@ -3927,7 +4156,7 @@
         <v>119</v>
       </c>
       <c r="C86" s="33"/>
-      <c r="D86" s="66"/>
+      <c r="D86" s="65"/>
       <c r="E86" s="34"/>
     </row>
     <row r="87" spans="2:5">
@@ -3935,7 +4164,7 @@
         <v>120</v>
       </c>
       <c r="C87" s="33"/>
-      <c r="D87" s="66" t="s">
+      <c r="D87" s="65" t="s">
         <v>121</v>
       </c>
       <c r="E87" s="34"/>
@@ -3945,7 +4174,7 @@
         <v>122</v>
       </c>
       <c r="C88" s="33"/>
-      <c r="D88" s="66"/>
+      <c r="D88" s="65"/>
       <c r="E88" s="34"/>
     </row>
     <row r="89" spans="2:5">
@@ -3953,7 +4182,7 @@
         <v>123</v>
       </c>
       <c r="C89" s="33"/>
-      <c r="D89" s="66" t="s">
+      <c r="D89" s="65" t="s">
         <v>124</v>
       </c>
       <c r="E89" s="34"/>
@@ -3963,7 +4192,7 @@
         <v>125</v>
       </c>
       <c r="C90" s="33"/>
-      <c r="D90" s="66"/>
+      <c r="D90" s="65"/>
       <c r="E90" s="34"/>
     </row>
     <row r="91" spans="2:5">
@@ -3971,7 +4200,7 @@
         <v>126</v>
       </c>
       <c r="C91" s="33"/>
-      <c r="D91" s="66"/>
+      <c r="D91" s="65"/>
       <c r="E91" s="34"/>
     </row>
     <row r="92" spans="2:5">
@@ -3979,7 +4208,7 @@
         <v>127</v>
       </c>
       <c r="C92" s="33"/>
-      <c r="D92" s="66"/>
+      <c r="D92" s="65"/>
       <c r="E92" s="34"/>
     </row>
     <row r="93" spans="2:5">
@@ -3987,7 +4216,7 @@
         <v>128</v>
       </c>
       <c r="C93" s="33"/>
-      <c r="D93" s="66"/>
+      <c r="D93" s="65"/>
       <c r="E93" s="34"/>
     </row>
     <row r="94" spans="2:5">
@@ -4003,7 +4232,7 @@
         <v>130</v>
       </c>
       <c r="C95" s="33"/>
-      <c r="D95" s="66"/>
+      <c r="D95" s="65"/>
       <c r="E95" s="34"/>
     </row>
     <row r="96" spans="2:5" ht="30">
@@ -4011,7 +4240,7 @@
         <v>131</v>
       </c>
       <c r="C96" s="33"/>
-      <c r="D96" s="66"/>
+      <c r="D96" s="65"/>
       <c r="E96" s="34"/>
     </row>
     <row r="97" spans="2:5">
@@ -4019,7 +4248,7 @@
         <v>132</v>
       </c>
       <c r="C97" s="33"/>
-      <c r="D97" s="66"/>
+      <c r="D97" s="65"/>
       <c r="E97" s="34"/>
     </row>
     <row r="98" spans="2:5">
@@ -4027,7 +4256,7 @@
         <v>133</v>
       </c>
       <c r="C98" s="33"/>
-      <c r="D98" s="66"/>
+      <c r="D98" s="65"/>
       <c r="E98" s="34"/>
     </row>
     <row r="99" spans="2:5">
@@ -4035,7 +4264,7 @@
         <v>134</v>
       </c>
       <c r="C99" s="33"/>
-      <c r="D99" s="66"/>
+      <c r="D99" s="65"/>
       <c r="E99" s="34"/>
     </row>
     <row r="100" spans="2:5">
@@ -4053,7 +4282,7 @@
         <v>137</v>
       </c>
       <c r="C101" s="33"/>
-      <c r="D101" s="66"/>
+      <c r="D101" s="65"/>
       <c r="E101" s="34"/>
     </row>
     <row r="102" spans="2:5">
@@ -4061,7 +4290,7 @@
         <v>138</v>
       </c>
       <c r="C102" s="33"/>
-      <c r="D102" s="66"/>
+      <c r="D102" s="65"/>
       <c r="E102" s="34"/>
     </row>
     <row r="103" spans="2:5">
@@ -4077,7 +4306,7 @@
         <v>140</v>
       </c>
       <c r="C104" s="33"/>
-      <c r="D104" s="66"/>
+      <c r="D104" s="65"/>
       <c r="E104" s="34"/>
     </row>
     <row r="105" spans="2:5">
@@ -4085,7 +4314,7 @@
         <v>141</v>
       </c>
       <c r="C105" s="33"/>
-      <c r="D105" s="66"/>
+      <c r="D105" s="65"/>
       <c r="E105" s="34"/>
     </row>
     <row r="106" spans="2:5">
@@ -4101,7 +4330,7 @@
         <v>143</v>
       </c>
       <c r="C107" s="33"/>
-      <c r="D107" s="66"/>
+      <c r="D107" s="65"/>
       <c r="E107" s="34"/>
     </row>
     <row r="108" spans="2:5">
@@ -4109,7 +4338,7 @@
         <v>144</v>
       </c>
       <c r="C108" s="33"/>
-      <c r="D108" s="66"/>
+      <c r="D108" s="65"/>
       <c r="E108" s="34"/>
     </row>
     <row r="109" spans="2:5">
@@ -4135,7 +4364,7 @@
         <v>148</v>
       </c>
       <c r="C111" s="33"/>
-      <c r="D111" s="66"/>
+      <c r="D111" s="65"/>
       <c r="E111" s="34"/>
     </row>
     <row r="112" spans="2:5">
@@ -4143,7 +4372,7 @@
         <v>149</v>
       </c>
       <c r="C112" s="33"/>
-      <c r="D112" s="66"/>
+      <c r="D112" s="65"/>
       <c r="E112" s="34"/>
     </row>
     <row r="113" spans="2:5" ht="30">
@@ -4151,7 +4380,7 @@
         <v>150</v>
       </c>
       <c r="C113" s="33"/>
-      <c r="D113" s="66"/>
+      <c r="D113" s="65"/>
       <c r="E113" s="34"/>
     </row>
     <row r="114" spans="2:5">
@@ -4159,7 +4388,7 @@
         <v>151</v>
       </c>
       <c r="C114" s="33"/>
-      <c r="D114" s="66" t="s">
+      <c r="D114" s="65" t="s">
         <v>152</v>
       </c>
       <c r="E114" s="34"/>
@@ -4169,7 +4398,7 @@
         <v>153</v>
       </c>
       <c r="C115" s="33"/>
-      <c r="D115" s="66"/>
+      <c r="D115" s="65"/>
       <c r="E115" s="34"/>
     </row>
     <row r="116" spans="2:5" ht="30">
@@ -4177,7 +4406,7 @@
         <v>154</v>
       </c>
       <c r="C116" s="33"/>
-      <c r="D116" s="66" t="s">
+      <c r="D116" s="65" t="s">
         <v>155</v>
       </c>
       <c r="E116" s="34"/>
@@ -4187,7 +4416,7 @@
         <v>156</v>
       </c>
       <c r="C117" s="33"/>
-      <c r="D117" s="66" t="s">
+      <c r="D117" s="65" t="s">
         <v>157</v>
       </c>
       <c r="E117" s="34"/>
@@ -4207,7 +4436,7 @@
         <v>160</v>
       </c>
       <c r="C119" s="33"/>
-      <c r="D119" s="66"/>
+      <c r="D119" s="65"/>
       <c r="E119" s="34"/>
     </row>
     <row r="120" spans="2:5" ht="30">
@@ -4215,7 +4444,7 @@
         <v>161</v>
       </c>
       <c r="C120" s="33"/>
-      <c r="D120" s="66" t="s">
+      <c r="D120" s="65" t="s">
         <v>162</v>
       </c>
       <c r="E120" s="34"/>
@@ -4225,7 +4454,7 @@
         <v>163</v>
       </c>
       <c r="C121" s="33"/>
-      <c r="D121" s="66"/>
+      <c r="D121" s="65"/>
       <c r="E121" s="34"/>
     </row>
     <row r="122" spans="2:5" ht="30">
@@ -4251,7 +4480,7 @@
         <v>167</v>
       </c>
       <c r="C124" s="33"/>
-      <c r="D124" s="66" t="s">
+      <c r="D124" s="65" t="s">
         <v>168</v>
       </c>
       <c r="E124" s="34"/>
@@ -4261,7 +4490,7 @@
         <v>169</v>
       </c>
       <c r="C125" s="33"/>
-      <c r="D125" s="66" t="s">
+      <c r="D125" s="65" t="s">
         <v>168</v>
       </c>
       <c r="E125" s="34"/>
@@ -4271,7 +4500,7 @@
         <v>170</v>
       </c>
       <c r="C126" s="33"/>
-      <c r="D126" s="66" t="s">
+      <c r="D126" s="65" t="s">
         <v>171</v>
       </c>
       <c r="E126" s="34"/>
@@ -4281,7 +4510,7 @@
         <v>172</v>
       </c>
       <c r="C127" s="33"/>
-      <c r="D127" s="66" t="s">
+      <c r="D127" s="65" t="s">
         <v>173</v>
       </c>
       <c r="E127" s="34"/>
@@ -4291,7 +4520,7 @@
         <v>174</v>
       </c>
       <c r="C128" s="33"/>
-      <c r="D128" s="66"/>
+      <c r="D128" s="65"/>
       <c r="E128" s="34"/>
     </row>
     <row r="129" spans="1:6">
@@ -4299,7 +4528,7 @@
         <v>175</v>
       </c>
       <c r="C129" s="33"/>
-      <c r="D129" s="66" t="s">
+      <c r="D129" s="65" t="s">
         <v>176</v>
       </c>
       <c r="E129" s="34"/>
@@ -4327,7 +4556,7 @@
         <v>179</v>
       </c>
       <c r="C132" s="33"/>
-      <c r="D132" s="66"/>
+      <c r="D132" s="65"/>
       <c r="E132" s="34"/>
     </row>
     <row r="133" spans="1:6">
@@ -4335,7 +4564,7 @@
         <v>180</v>
       </c>
       <c r="C133" s="33"/>
-      <c r="D133" s="66"/>
+      <c r="D133" s="65"/>
       <c r="E133" s="34"/>
     </row>
     <row r="134" spans="1:6">
@@ -4343,7 +4572,7 @@
         <v>181</v>
       </c>
       <c r="C134" s="33"/>
-      <c r="D134" s="66"/>
+      <c r="D134" s="65"/>
       <c r="E134" s="34"/>
     </row>
     <row r="138" spans="1:6" ht="30">
@@ -4360,21 +4589,21 @@
         <v>184</v>
       </c>
       <c r="C139" s="33"/>
-      <c r="D139" s="66"/>
+      <c r="D139" s="65"/>
     </row>
     <row r="140" spans="1:6">
       <c r="B140" s="32" t="s">
         <v>185</v>
       </c>
       <c r="C140" s="33"/>
-      <c r="D140" s="66"/>
+      <c r="D140" s="65"/>
     </row>
     <row r="141" spans="1:6" ht="30">
       <c r="B141" s="41" t="s">
         <v>186</v>
       </c>
       <c r="C141" s="33"/>
-      <c r="D141" s="66" t="s">
+      <c r="D141" s="65" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4383,35 +4612,35 @@
         <v>188</v>
       </c>
       <c r="C142" s="33"/>
-      <c r="D142" s="66"/>
+      <c r="D142" s="65"/>
     </row>
     <row r="143" spans="1:6">
       <c r="B143" s="32" t="s">
         <v>189</v>
       </c>
       <c r="C143" s="33"/>
-      <c r="D143" s="66"/>
+      <c r="D143" s="65"/>
     </row>
     <row r="144" spans="1:6">
       <c r="B144" s="32" t="s">
         <v>190</v>
       </c>
       <c r="C144" s="33"/>
-      <c r="D144" s="66"/>
+      <c r="D144" s="65"/>
     </row>
     <row r="145" spans="2:4">
       <c r="B145" s="32" t="s">
         <v>191</v>
       </c>
       <c r="C145" s="33"/>
-      <c r="D145" s="66"/>
+      <c r="D145" s="65"/>
     </row>
     <row r="146" spans="2:4">
       <c r="B146" s="41" t="s">
         <v>192</v>
       </c>
       <c r="C146" s="33"/>
-      <c r="D146" s="66" t="s">
+      <c r="D146" s="65" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4420,42 +4649,42 @@
         <v>194</v>
       </c>
       <c r="C147" s="33"/>
-      <c r="D147" s="66"/>
+      <c r="D147" s="65"/>
     </row>
     <row r="148" spans="2:4">
       <c r="B148" s="41" t="s">
         <v>195</v>
       </c>
       <c r="C148" s="33"/>
-      <c r="D148" s="66"/>
+      <c r="D148" s="65"/>
     </row>
     <row r="149" spans="2:4">
       <c r="B149" s="41" t="s">
         <v>196</v>
       </c>
       <c r="C149" s="33"/>
-      <c r="D149" s="66"/>
+      <c r="D149" s="65"/>
     </row>
     <row r="150" spans="2:4">
       <c r="B150" s="41" t="s">
         <v>197</v>
       </c>
       <c r="C150" s="33"/>
-      <c r="D150" s="66"/>
+      <c r="D150" s="65"/>
     </row>
     <row r="151" spans="2:4">
       <c r="B151" s="41" t="s">
         <v>198</v>
       </c>
       <c r="C151" s="33"/>
-      <c r="D151" s="66"/>
+      <c r="D151" s="65"/>
     </row>
     <row r="152" spans="2:4">
       <c r="B152" s="41" t="s">
         <v>199</v>
       </c>
       <c r="C152" s="33"/>
-      <c r="D152" s="66"/>
+      <c r="D152" s="65"/>
     </row>
     <row r="155" spans="2:4" ht="18.75">
       <c r="B155" s="50" t="s">
@@ -4495,14 +4724,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="2"/>
@@ -4526,32 +4755,32 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="52" t="s">
@@ -4560,7 +4789,7 @@
       <c r="B10" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="67" t="s">
         <v>200</v>
       </c>
       <c r="D10" s="52" t="s">
@@ -4570,7 +4799,7 @@
     <row r="11" spans="1:7">
       <c r="A11" s="53"/>
       <c r="B11" s="54"/>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="68" t="s">
         <v>203</v>
       </c>
       <c r="D11" s="55"/>
@@ -4580,7 +4809,7 @@
       <c r="B12" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="69"/>
+      <c r="C12" s="68"/>
       <c r="D12" s="55"/>
     </row>
     <row r="13" spans="1:7">
@@ -4590,7 +4819,7 @@
       <c r="B13" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="68"/>
       <c r="D13" s="55"/>
     </row>
     <row r="14" spans="1:7">
@@ -4650,7 +4879,7 @@
       <c r="B19" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="C19" s="69"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="55"/>
     </row>
     <row r="20" spans="1:4">
@@ -4702,7 +4931,7 @@
       <c r="B25" s="54" t="s">
         <v>222</v>
       </c>
-      <c r="C25" s="69"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="56" t="s">
         <v>223</v>
       </c>
@@ -4748,7 +4977,7 @@
       <c r="B30" s="54" t="s">
         <v>227</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="68"/>
       <c r="D30" s="55"/>
     </row>
     <row r="31" spans="1:4">
@@ -4784,7 +5013,7 @@
       <c r="B34" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="C34" s="69"/>
+      <c r="C34" s="68"/>
       <c r="D34" s="55"/>
     </row>
     <row r="35" spans="1:4">
@@ -4828,7 +5057,7 @@
       <c r="B39" s="54" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="69"/>
+      <c r="C39" s="68"/>
       <c r="D39" s="56" t="s">
         <v>233</v>
       </c>
@@ -4866,7 +5095,7 @@
       <c r="B43" s="54" t="s">
         <v>236</v>
       </c>
-      <c r="C43" s="69"/>
+      <c r="C43" s="68"/>
       <c r="D43" s="56" t="s">
         <v>237</v>
       </c>
@@ -4940,7 +5169,7 @@
       <c r="B51" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="C51" s="69"/>
+      <c r="C51" s="68"/>
       <c r="D51" s="55"/>
     </row>
     <row r="52" spans="1:4">
@@ -4976,7 +5205,7 @@
       <c r="B55" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="C55" s="69"/>
+      <c r="C55" s="68"/>
       <c r="D55" s="56" t="s">
         <v>246</v>
       </c>
@@ -5012,7 +5241,7 @@
       <c r="B59" s="54" t="s">
         <v>248</v>
       </c>
-      <c r="C59" s="67"/>
+      <c r="C59" s="66"/>
       <c r="D59" s="56" t="s">
         <v>249</v>
       </c>
@@ -5022,7 +5251,7 @@
       <c r="B60" s="54" t="s">
         <v>250</v>
       </c>
-      <c r="C60" s="67"/>
+      <c r="C60" s="66"/>
       <c r="D60" s="56" t="s">
         <v>251</v>
       </c>
@@ -5032,7 +5261,7 @@
       <c r="B61" s="60" t="s">
         <v>252</v>
       </c>
-      <c r="C61" s="67"/>
+      <c r="C61" s="66"/>
       <c r="D61" s="56" t="s">
         <v>253</v>
       </c>
@@ -5042,7 +5271,7 @@
       <c r="B62" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="C62" s="69"/>
+      <c r="C62" s="68"/>
       <c r="D62" s="53"/>
     </row>
     <row r="63" spans="1:4">
@@ -5090,7 +5319,7 @@
       <c r="B67" s="61" t="s">
         <v>263</v>
       </c>
-      <c r="C67" s="69"/>
+      <c r="C67" s="68"/>
       <c r="D67" s="53"/>
     </row>
     <row r="68" spans="1:4">
@@ -5130,10 +5359,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5144,21 +5373,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="86"/>
+      <c r="A2" s="85"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="86"/>
+      <c r="A3" s="85"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="87"/>
+      <c r="A4" s="86"/>
       <c r="B4" t="s">
         <v>289</v>
       </c>
@@ -5170,306 +5399,594 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
     </row>
     <row r="6" spans="1:4" ht="90">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="102" t="s">
         <v>301</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>293</v>
       </c>
-      <c r="C6" s="89" t="s">
+      <c r="C6" s="88" t="s">
         <v>293</v>
       </c>
-      <c r="D6" s="90"/>
+      <c r="D6" s="89"/>
     </row>
     <row r="7" spans="1:4" ht="90">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="102" t="s">
         <v>294</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="91" t="s">
         <v>295</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="87" t="s">
         <v>295</v>
       </c>
-      <c r="D7" s="88" t="s">
+      <c r="D7" s="87" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="102" t="s">
         <v>296</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="91" t="s">
         <v>298</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="87" t="s">
         <v>298</v>
       </c>
-      <c r="D8" s="90"/>
+      <c r="D8" s="89"/>
     </row>
     <row r="9" spans="1:4" ht="45">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
     </row>
     <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="104" t="s">
         <v>300</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
     </row>
     <row r="11" spans="1:4" ht="45">
-      <c r="A11" s="86" t="s">
+      <c r="A11" s="102" t="s">
         <v>308</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="91" t="s">
         <v>309</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="87" t="s">
         <v>309</v>
       </c>
-      <c r="D11" s="88"/>
+      <c r="D11" s="87"/>
     </row>
     <row r="12" spans="1:4" ht="45">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="87" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="75">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="102" t="s">
         <v>306</v>
       </c>
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="91" t="s">
         <v>310</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="87" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="104" t="s">
         <v>299</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
     </row>
     <row r="15" spans="1:4" ht="105">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="102" t="s">
         <v>292</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="91" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="87" t="s">
         <v>303</v>
       </c>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="87" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="87" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="90">
-      <c r="A17" s="86" t="s">
+      <c r="A17" s="102" t="s">
         <v>306</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="91" t="s">
         <v>307</v>
       </c>
-      <c r="C17" s="88" t="s">
+      <c r="C17" s="87" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="75">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="103" t="s">
         <v>280</v>
       </c>
+      <c r="B18" s="102"/>
+      <c r="C18" s="102"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="104" t="s">
         <v>281</v>
       </c>
-      <c r="C19" s="88"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="87"/>
     </row>
     <row r="20" spans="1:4" ht="120">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="102" t="s">
+        <v>350</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>314</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>314</v>
+      </c>
+      <c r="D20" s="100" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="104" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="100"/>
+    </row>
+    <row r="22" spans="1:4" ht="105">
+      <c r="A22" s="102" t="s">
         <v>311</v>
       </c>
-      <c r="B20" s="92" t="s">
-        <v>314</v>
-      </c>
-      <c r="C20" s="88" t="s">
-        <v>314</v>
-      </c>
-      <c r="D20" s="102" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="93" t="s">
-        <v>278</v>
-      </c>
-      <c r="D21" s="102"/>
-    </row>
-    <row r="22" spans="1:4" ht="105">
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="91" t="s">
         <v>313</v>
       </c>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="87" t="s">
         <v>313</v>
       </c>
-      <c r="D22" s="102"/>
+      <c r="D22" s="100"/>
     </row>
     <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="103" t="s">
         <v>282</v>
       </c>
-      <c r="D23" s="86"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="D24" s="86"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="D25" s="86"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="D26" s="86"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="D27" s="86"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="D28" s="86"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="D29" s="86"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="D30" s="86"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="B31" s="90"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="B32" s="90"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="B33" s="90"/>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="86"/>
-      <c r="B34" s="90"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="90"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="86"/>
-      <c r="B35" s="90"/>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="86"/>
-      <c r="B36" s="90"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="86"/>
-      <c r="B37" s="90"/>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="B38" s="90"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-    </row>
-    <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="62" t="s">
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="85"/>
+    </row>
+    <row r="24" spans="1:4" ht="60">
+      <c r="A24" s="104" t="s">
+        <v>315</v>
+      </c>
+      <c r="B24" s="102"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="85"/>
+    </row>
+    <row r="25" spans="1:4" ht="135">
+      <c r="A25" s="102" t="s">
+        <v>317</v>
+      </c>
+      <c r="B25" s="105" t="s">
+        <v>316</v>
+      </c>
+      <c r="C25" s="102" t="s">
+        <v>316</v>
+      </c>
+      <c r="D25" s="85"/>
+    </row>
+    <row r="26" spans="1:4" ht="75">
+      <c r="A26" s="102" t="s">
+        <v>318</v>
+      </c>
+      <c r="B26" s="105" t="s">
+        <v>319</v>
+      </c>
+      <c r="C26" s="102" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" s="85"/>
+    </row>
+    <row r="27" spans="1:4" ht="45">
+      <c r="A27" s="102" t="s">
+        <v>320</v>
+      </c>
+      <c r="B27" s="105" t="s">
+        <v>321</v>
+      </c>
+      <c r="C27" s="102" t="s">
+        <v>321</v>
+      </c>
+      <c r="D27" s="85"/>
+    </row>
+    <row r="28" spans="1:4" ht="90">
+      <c r="A28" s="102" t="s">
+        <v>322</v>
+      </c>
+      <c r="B28" s="105" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" s="102" t="s">
+        <v>319</v>
+      </c>
+      <c r="D28" s="85"/>
+    </row>
+    <row r="29" spans="1:4" ht="45">
+      <c r="A29" s="102" t="s">
+        <v>320</v>
+      </c>
+      <c r="B29" s="105" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="102" t="s">
+        <v>321</v>
+      </c>
+      <c r="D29" s="85"/>
+    </row>
+    <row r="30" spans="1:4" ht="90">
+      <c r="A30" s="102" t="s">
+        <v>323</v>
+      </c>
+      <c r="B30" s="105" t="s">
+        <v>324</v>
+      </c>
+      <c r="C30" s="102" t="s">
+        <v>324</v>
+      </c>
+      <c r="D30" s="85"/>
+    </row>
+    <row r="31" spans="1:4" ht="75">
+      <c r="A31" s="102" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" s="91" t="s">
+        <v>326</v>
+      </c>
+      <c r="C31" s="87" t="s">
+        <v>326</v>
+      </c>
+      <c r="D31" s="89"/>
+    </row>
+    <row r="32" spans="1:4" ht="30">
+      <c r="A32" s="102" t="s">
+        <v>341</v>
+      </c>
+      <c r="B32" s="91" t="s">
+        <v>342</v>
+      </c>
+      <c r="C32" s="87" t="s">
+        <v>342</v>
+      </c>
+      <c r="D32" s="89"/>
+    </row>
+    <row r="33" spans="1:4" ht="60">
+      <c r="A33" s="104" t="s">
+        <v>330</v>
+      </c>
+      <c r="B33" s="102"/>
+      <c r="C33" s="102"/>
+      <c r="D33" s="89"/>
+    </row>
+    <row r="34" spans="1:4" ht="90">
+      <c r="A34" s="102"/>
+      <c r="B34" s="105" t="s">
+        <v>332</v>
+      </c>
+      <c r="C34" s="102" t="s">
+        <v>332</v>
+      </c>
+      <c r="D34" s="89"/>
+    </row>
+    <row r="35" spans="1:4" ht="120">
+      <c r="A35" s="102" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" s="105" t="s">
+        <v>331</v>
+      </c>
+      <c r="C35" s="102" t="s">
+        <v>331</v>
+      </c>
+      <c r="D35" s="89"/>
+    </row>
+    <row r="36" spans="1:4" ht="30">
+      <c r="A36" s="103" t="s">
         <v>283</v>
       </c>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-    </row>
-    <row r="40" spans="1:4" ht="45">
-      <c r="A40" s="62" t="s">
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+    </row>
+    <row r="37" spans="1:4" ht="120">
+      <c r="A37" s="102" t="s">
+        <v>327</v>
+      </c>
+      <c r="B37" s="105" t="s">
+        <v>328</v>
+      </c>
+      <c r="C37" s="102" t="s">
+        <v>328</v>
+      </c>
+      <c r="D37" s="89"/>
+    </row>
+    <row r="38" spans="1:4" ht="120">
+      <c r="A38" s="102" t="s">
+        <v>329</v>
+      </c>
+      <c r="B38" s="105" t="s">
+        <v>328</v>
+      </c>
+      <c r="C38" s="102" t="s">
+        <v>328</v>
+      </c>
+      <c r="D38" s="89"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="102"/>
+      <c r="B39" s="102"/>
+      <c r="C39" s="102"/>
+      <c r="D39" s="89"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="102"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="89"/>
+    </row>
+    <row r="41" spans="1:4" ht="45">
+      <c r="A41" s="103" t="s">
         <v>284</v>
       </c>
-      <c r="B40" s="90"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
-    </row>
-    <row r="41" spans="1:4" ht="30">
-      <c r="A41" s="62" t="s">
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="89"/>
+    </row>
+    <row r="42" spans="1:4" ht="105">
+      <c r="A42" s="102" t="s">
+        <v>334</v>
+      </c>
+      <c r="B42" s="105" t="s">
+        <v>335</v>
+      </c>
+      <c r="C42" s="102" t="s">
+        <v>335</v>
+      </c>
+      <c r="D42" s="89"/>
+    </row>
+    <row r="43" spans="1:4" ht="105">
+      <c r="A43" s="102" t="s">
+        <v>336</v>
+      </c>
+      <c r="B43" s="91" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" s="87" t="s">
+        <v>337</v>
+      </c>
+      <c r="D43" s="89"/>
+    </row>
+    <row r="44" spans="1:4" ht="30">
+      <c r="A44" s="102" t="s">
+        <v>341</v>
+      </c>
+      <c r="B44" s="91" t="s">
+        <v>342</v>
+      </c>
+      <c r="C44" s="87" t="s">
+        <v>342</v>
+      </c>
+      <c r="D44" s="89"/>
+    </row>
+    <row r="45" spans="1:4" ht="75">
+      <c r="A45" s="102" t="s">
+        <v>355</v>
+      </c>
+      <c r="B45" s="105" t="s">
+        <v>335</v>
+      </c>
+      <c r="C45" s="102" t="s">
+        <v>335</v>
+      </c>
+      <c r="D45" s="85"/>
+    </row>
+    <row r="46" spans="1:4" ht="45">
+      <c r="B46" s="105" t="s">
+        <v>356</v>
+      </c>
+      <c r="C46" s="102" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30">
+      <c r="A47" s="103" t="s">
         <v>285</v>
       </c>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-    </row>
-    <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="62" t="s">
+      <c r="B47" s="89"/>
+      <c r="C47" s="89"/>
+    </row>
+    <row r="48" spans="1:4" ht="60">
+      <c r="A48" s="102" t="s">
+        <v>338</v>
+      </c>
+      <c r="B48" s="105" t="s">
+        <v>339</v>
+      </c>
+      <c r="C48" s="102" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="90">
+      <c r="A49" s="102" t="s">
+        <v>336</v>
+      </c>
+      <c r="B49" s="91" t="s">
+        <v>340</v>
+      </c>
+      <c r="C49" s="87" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30">
+      <c r="A50" s="102" t="s">
+        <v>341</v>
+      </c>
+      <c r="B50" s="91" t="s">
+        <v>342</v>
+      </c>
+      <c r="C50" s="87" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="60">
+      <c r="A51" s="102" t="s">
+        <v>353</v>
+      </c>
+      <c r="B51" s="105" t="s">
+        <v>339</v>
+      </c>
+      <c r="C51" s="102" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="45">
+      <c r="B52" s="105" t="s">
+        <v>354</v>
+      </c>
+      <c r="C52" s="102" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30">
+      <c r="A53" s="103" t="s">
         <v>286</v>
       </c>
-      <c r="B42" s="90"/>
-      <c r="C42" s="90"/>
-      <c r="D42" s="90"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="62" t="s">
+      <c r="B53" s="85"/>
+      <c r="C53" s="85"/>
+    </row>
+    <row r="54" spans="1:4" ht="75">
+      <c r="A54" s="102" t="s">
+        <v>343</v>
+      </c>
+      <c r="B54" s="105" t="s">
+        <v>344</v>
+      </c>
+      <c r="C54" s="102" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="45">
+      <c r="A55" s="102" t="s">
+        <v>345</v>
+      </c>
+      <c r="B55" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="C55" s="87" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30">
+      <c r="A56" s="102" t="s">
+        <v>341</v>
+      </c>
+      <c r="B56" s="91" t="s">
+        <v>342</v>
+      </c>
+      <c r="C56" s="87" t="s">
+        <v>342</v>
+      </c>
+      <c r="D56" s="62"/>
+    </row>
+    <row r="57" spans="1:4" ht="60">
+      <c r="A57" s="102" t="s">
+        <v>351</v>
+      </c>
+      <c r="B57" s="105" t="s">
+        <v>344</v>
+      </c>
+      <c r="C57" s="102" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="45">
+      <c r="B58" s="105" t="s">
+        <v>352</v>
+      </c>
+      <c r="C58" s="102" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="103" t="s">
         <v>287</v>
       </c>
-      <c r="B43" s="90"/>
-      <c r="C43" s="90"/>
-      <c r="D43" s="90"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="62" t="s">
+      <c r="B60" s="85"/>
+      <c r="C60" s="85"/>
+    </row>
+    <row r="61" spans="1:4" ht="90">
+      <c r="A61" s="102" t="s">
+        <v>347</v>
+      </c>
+      <c r="B61" s="101" t="s">
+        <v>348</v>
+      </c>
+      <c r="C61" s="85" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="60">
+      <c r="B62" s="105" t="s">
+        <v>349</v>
+      </c>
+      <c r="C62" s="102" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="103" t="s">
         <v>288</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="90"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="D45" s="86"/>
+      <c r="B63" s="85"/>
+      <c r="C63" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add forgot case for Nesting level
</commit_message>
<xml_diff>
--- a/iSpring/TestCase.xlsx
+++ b/iSpring/TestCase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
   <si>
     <t>Изменение заголовка слайда</t>
   </si>
@@ -424,6 +424,24 @@
   </si>
   <si>
     <t>Шаги\Название</t>
+  </si>
+  <si>
+    <t>Группировка слайдов</t>
+  </si>
+  <si>
+    <t>Нажимаем на стрелку вправо у слайда</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Выделенный слайд сдвигается вправо и соединяются линиями со слайдом "родителем"(тот что выше)</t>
+  </si>
+  <si>
+    <t>Тестировалось на презентации без группировки слайдов</t>
+  </si>
+  <si>
+    <t>Нажимаем на стрелку влево у слайда</t>
+  </si>
+  <si>
+    <t>Слайд возвращается в исходное положение</t>
   </si>
 </sst>
 </file>
@@ -523,7 +541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -544,6 +562,37 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -677,141 +726,168 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent6 2" xfId="3"/>
@@ -1325,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1338,1040 +1414,1067 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="53" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" ht="90">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4" ht="90">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="31" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90.75" thickBot="1">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A9" s="24"/>
-      <c r="B9" s="42" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A10" s="24"/>
-      <c r="B10" s="46" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" ht="45">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" ht="45">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" ht="75.75" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="24"/>
-      <c r="B14" s="46" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" ht="105">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" ht="90.75" thickBot="1">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" ht="75" customHeight="1" thickBot="1">
-      <c r="A18" s="24"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A19" s="24"/>
-      <c r="B19" s="46" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" ht="120.75" thickBot="1">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="38" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A21" s="50"/>
-      <c r="B21" s="46" t="s">
+      <c r="A21" s="22"/>
+      <c r="B21" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="51"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="39"/>
     </row>
     <row r="22" spans="1:4" ht="105.75" thickBot="1">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="38" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A23" s="24"/>
-      <c r="B23" s="42" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
     </row>
     <row r="24" spans="1:4" ht="60" customHeight="1" thickBot="1">
-      <c r="A24" s="24"/>
-      <c r="B24" s="46" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="37"/>
     </row>
     <row r="25" spans="1:4" ht="135">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="36"/>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" spans="1:4" ht="75">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="36"/>
+      <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:4" ht="45">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="36"/>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" spans="1:4" ht="90">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="36"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:4" ht="45">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:4" ht="90">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="36"/>
+      <c r="D30" s="41"/>
     </row>
     <row r="31" spans="1:4" ht="75">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="31"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="31"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="60" customHeight="1" thickBot="1">
-      <c r="A33" s="24"/>
-      <c r="B33" s="46" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
     </row>
     <row r="34" spans="1:4" ht="90">
-      <c r="A34" s="19"/>
-      <c r="B34" s="35" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="31"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" ht="120.75" thickBot="1">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="31"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="42" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="34"/>
     </row>
     <row r="37" spans="1:4" ht="120">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="31"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" ht="120">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="31"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="19"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="31"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A40" s="19"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="31"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="42" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="28"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="34"/>
     </row>
     <row r="42" spans="1:4" ht="105">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="31"/>
+      <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:4" ht="105">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="31"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:4" ht="30">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="31"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:4" ht="75">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="36"/>
+      <c r="D45" s="41"/>
     </row>
     <row r="46" spans="1:4" ht="45.75" thickBot="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="35" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="11"/>
+      <c r="D46" s="20"/>
     </row>
     <row r="47" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A47" s="24"/>
-      <c r="B47" s="42" t="s">
+      <c r="A47" s="17"/>
+      <c r="B47" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="28"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="34"/>
     </row>
     <row r="48" spans="1:4" ht="60">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="11"/>
+      <c r="D48" s="20"/>
     </row>
     <row r="49" spans="1:4" ht="90">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="C49" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="11"/>
+      <c r="D49" s="20"/>
     </row>
     <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="11"/>
+      <c r="D50" s="20"/>
     </row>
     <row r="51" spans="1:4" ht="60">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="11"/>
+      <c r="D51" s="20"/>
     </row>
     <row r="52" spans="1:4" ht="45.75" thickBot="1">
-      <c r="A52" s="20"/>
-      <c r="B52" s="35" t="s">
+      <c r="A52" s="13"/>
+      <c r="B52" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D52" s="11"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A53" s="24"/>
-      <c r="B53" s="42" t="s">
+      <c r="A53" s="17"/>
+      <c r="B53" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="48"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="43"/>
     </row>
     <row r="54" spans="1:4" ht="75">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="11"/>
+      <c r="D54" s="20"/>
     </row>
     <row r="55" spans="1:4" ht="45">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="33" t="s">
+      <c r="C55" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D55" s="11"/>
+      <c r="D55" s="20"/>
     </row>
     <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="33" t="s">
+      <c r="C56" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="37"/>
+      <c r="D56" s="20"/>
     </row>
     <row r="57" spans="1:4" ht="60">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D57" s="11"/>
+      <c r="D57" s="20"/>
     </row>
     <row r="58" spans="1:4" ht="45.75" thickBot="1">
-      <c r="A58" s="20"/>
-      <c r="B58" s="35" t="s">
+      <c r="A58" s="13"/>
+      <c r="B58" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D58" s="11"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A59" s="24"/>
-      <c r="B59" s="42" t="s">
+      <c r="A59" s="17"/>
+      <c r="B59" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="28"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="34"/>
     </row>
     <row r="60" spans="1:4" ht="90">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="11"/>
+      <c r="D60" s="20"/>
     </row>
     <row r="61" spans="1:4" ht="60.75" thickBot="1">
-      <c r="A61" s="20"/>
-      <c r="B61" s="40" t="s">
+      <c r="A61" s="13"/>
+      <c r="B61" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="18"/>
+      <c r="D61" s="46"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A62" s="24"/>
-      <c r="B62" s="42" t="s">
+      <c r="A62" s="17"/>
+      <c r="B62" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="28"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="34"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A63" s="21"/>
-      <c r="B63" s="43" t="s">
+      <c r="A63" s="14"/>
+      <c r="B63" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="45"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="49"/>
     </row>
     <row r="64" spans="1:4" ht="90">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="11"/>
+      <c r="D64" s="20"/>
     </row>
     <row r="65" spans="1:4" ht="45">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="11"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="20"/>
     </row>
     <row r="66" spans="1:4" ht="60">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="11"/>
+      <c r="D66" s="20"/>
     </row>
     <row r="67" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D67" s="11"/>
+      <c r="D67" s="20"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A68" s="24"/>
-      <c r="B68" s="46" t="s">
+      <c r="A68" s="17"/>
+      <c r="B68" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="25"/>
-      <c r="D68" s="26"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
     </row>
     <row r="69" spans="1:4" ht="60">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D69" s="11"/>
+      <c r="D69" s="20"/>
     </row>
     <row r="70" spans="1:4" ht="30">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="11"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="20"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D71" s="11"/>
+      <c r="D71" s="20"/>
     </row>
     <row r="72" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D72" s="11"/>
+      <c r="D72" s="20"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A73" s="24"/>
-      <c r="B73" s="46" t="s">
+      <c r="A73" s="17"/>
+      <c r="B73" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C73" s="25"/>
-      <c r="D73" s="26"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="37"/>
     </row>
     <row r="74" spans="1:4" ht="90">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D74" s="11"/>
+      <c r="D74" s="20"/>
     </row>
     <row r="75" spans="1:4" ht="45">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="11"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="20"/>
     </row>
     <row r="76" spans="1:4" ht="30">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D76" s="11"/>
+      <c r="D76" s="20"/>
     </row>
     <row r="77" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D77" s="11"/>
+      <c r="D77" s="20"/>
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A78" s="24"/>
-      <c r="B78" s="46" t="s">
+      <c r="A78" s="17"/>
+      <c r="B78" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C78" s="25"/>
-      <c r="D78" s="26"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="37"/>
     </row>
     <row r="79" spans="1:4" ht="30" customHeight="1">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C79" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D79" s="11"/>
+      <c r="D79" s="20"/>
     </row>
     <row r="80" spans="1:4" ht="30">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D80" s="11"/>
+      <c r="D80" s="20"/>
     </row>
     <row r="81" spans="1:4" ht="45.75" thickBot="1">
-      <c r="A81" s="19"/>
-      <c r="B81" s="9" t="s">
+      <c r="A81" s="12"/>
+      <c r="B81" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D81" s="11"/>
+      <c r="D81" s="20"/>
     </row>
     <row r="82" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A82" s="24"/>
-      <c r="B82" s="46" t="s">
+      <c r="A82" s="17"/>
+      <c r="B82" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="37"/>
     </row>
     <row r="83" spans="1:4" ht="60.75" thickBot="1">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="11"/>
+      <c r="D83" s="20"/>
     </row>
     <row r="84" spans="1:4" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A84" s="24"/>
-      <c r="B84" s="46" t="s">
+      <c r="A84" s="17"/>
+      <c r="B84" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="25"/>
-      <c r="D84" s="26"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="37"/>
     </row>
     <row r="85" spans="1:4" ht="30" customHeight="1">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="20"/>
     </row>
     <row r="86" spans="1:4" ht="45">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C86" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D86" s="11"/>
+      <c r="D86" s="20"/>
     </row>
     <row r="87" spans="1:4" ht="45.75" thickBot="1">
-      <c r="A87" s="19" t="s">
+      <c r="A87" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C87" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D87" s="11"/>
+      <c r="D87" s="20"/>
     </row>
     <row r="88" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A88" s="24"/>
-      <c r="B88" s="46" t="s">
+      <c r="A88" s="17"/>
+      <c r="B88" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="C88" s="25"/>
-      <c r="D88" s="26"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="37"/>
     </row>
     <row r="89" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A89" s="19" t="s">
+      <c r="A89" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C89" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D89" s="11"/>
+      <c r="D89" s="20"/>
     </row>
     <row r="90" spans="1:4" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A90" s="24"/>
-      <c r="B90" s="46" t="s">
+      <c r="A90" s="17"/>
+      <c r="B90" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C90" s="25"/>
-      <c r="D90" s="26"/>
+      <c r="C90" s="36"/>
+      <c r="D90" s="37"/>
     </row>
     <row r="91" spans="1:4" ht="45" customHeight="1">
-      <c r="A91" s="22" t="s">
+      <c r="A91" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D91" s="11"/>
+      <c r="D91" s="20"/>
     </row>
     <row r="92" spans="1:4" ht="60.75" thickBot="1">
-      <c r="A92" s="22" t="s">
+      <c r="A92" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C92" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D92" s="11"/>
+      <c r="D92" s="20"/>
     </row>
     <row r="93" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A93" s="24"/>
-      <c r="B93" s="46" t="s">
+      <c r="A93" s="17"/>
+      <c r="B93" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="C93" s="25"/>
-      <c r="D93" s="26"/>
+      <c r="C93" s="36"/>
+      <c r="D93" s="37"/>
     </row>
     <row r="94" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C94" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D94" s="11"/>
+      <c r="D94" s="20"/>
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A95" s="24"/>
-      <c r="B95" s="46" t="s">
+      <c r="A95" s="17"/>
+      <c r="B95" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C95" s="25"/>
-      <c r="D95" s="26"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="37"/>
     </row>
     <row r="96" spans="1:4" ht="60">
-      <c r="A96" s="19" t="s">
+      <c r="A96" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D96" s="11"/>
+      <c r="D96" s="20"/>
     </row>
     <row r="97" spans="1:4" ht="45">
-      <c r="A97" s="19" t="s">
+      <c r="A97" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C97" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D97" s="11"/>
+      <c r="D97" s="20"/>
     </row>
     <row r="98" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A98" s="23" t="s">
+      <c r="A98" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="C98" s="17" t="s">
+      <c r="C98" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="18"/>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="5"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="5"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="4"/>
+      <c r="D98" s="46"/>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A100" s="57"/>
+      <c r="B100" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C100" s="60"/>
+      <c r="D100" s="61"/>
+    </row>
+    <row r="101" spans="1:4" ht="90.75" thickBot="1">
+      <c r="A101" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B101" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="C101" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D101" s="64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="45.75" thickBot="1">
+      <c r="A102" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C102" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D102" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
+    <mergeCell ref="B100:D100"/>
     <mergeCell ref="B84:D84"/>
     <mergeCell ref="B88:D88"/>
     <mergeCell ref="B90:D90"/>

</xml_diff>